<commit_message>
Test Torsion - config Diff out of Frame
</commit_message>
<xml_diff>
--- a/FR_Frame_Body/FR_A0100 (Frame)/Minimum Rules - Primary Structures.xlsx
+++ b/FR_Frame_Body/FR_A0100 (Frame)/Minimum Rules - Primary Structures.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calixthe\Desktop\EPSA\Gitkraken\STUF2020\STUF-2020\FR_Frame_Body\Frame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calixthe\Desktop\EPSA\Gitkraken\STUF2020\STUF-2020\FR_Frame_Body\FR_A0100 (Frame)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4902E464-0423-4806-A191-B39305875AC8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{575E58A5-A155-4AA1-B1CF-62E5F1C64EE8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="396" yWindow="684" windowWidth="21468" windowHeight="10872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Etude Structure Primaire" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="35">
   <si>
     <t>Minimum requirements of frame</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>Calixthe MATTEI</t>
-  </si>
-  <si>
-    <t>Sur cette image, il faut inverser la couleur des tubes jaunes et verts</t>
   </si>
   <si>
     <t>ULMTECHNOLOGIE</t>
@@ -389,14 +386,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -538,15 +535,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>453936</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>1235610</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>294188</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>129940</xdr:rowOff>
+      <xdr:colOff>60959</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -569,13 +566,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect r="43655" b="47121"/>
+        <a:srcRect t="3877" b="53127"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14409422" y="2852057"/>
-          <a:ext cx="6284595" cy="2938454"/>
+          <a:off x="15195450" y="2453640"/>
+          <a:ext cx="5271869" cy="2880360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -952,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="R53" sqref="Q50:R53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -974,26 +971,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="2" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="J3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="33" t="s">
+      <c r="K3" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H6" s="5" t="s">
@@ -1727,7 +1724,7 @@
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>22</v>
       </c>
@@ -1751,9 +1748,6 @@
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
-      <c r="L33" s="1" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="23"/>
@@ -1781,7 +1775,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B62" s="23"/>
       <c r="C62" s="23"/>
@@ -1797,10 +1791,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B64" s="23" t="s">
         <v>34</v>
-      </c>
-      <c r="B64" s="23" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2058,10 +2052,10 @@
   <sheetData>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
@@ -2245,7 +2239,7 @@
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="27">
         <v>20</v>
@@ -2271,7 +2265,7 @@
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="27">
         <v>20</v>
@@ -2470,11 +2464,11 @@
       <c r="J19" s="25"/>
     </row>
     <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="35" t="s">
-        <v>32</v>
+      <c r="A20" s="33" t="s">
+        <v>31</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" s="28">
         <v>25</v>
@@ -2502,7 +2496,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B21" s="26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" s="28">
         <v>25</v>
@@ -2674,7 +2668,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B28" s="26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28" s="28">
         <v>28</v>
@@ -2700,7 +2694,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B29" s="26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" s="28">
         <v>28</v>
@@ -2776,7 +2770,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B32" s="26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C32" s="28">
         <v>30</v>

</xml_diff>

<commit_message>
Maj pour Formation Frame
</commit_message>
<xml_diff>
--- a/FR_Frame_Body/FR_A0100 (Frame)/Minimum Rules - Primary Structures.xlsx
+++ b/FR_Frame_Body/FR_A0100 (Frame)/Minimum Rules - Primary Structures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calixthe\Desktop\EPSA\STUF-2020\FR_Frame_Body\FR_A0100 (Frame)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165305B3-EC8D-431A-BFDA-5508025FB3FA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CAD0B0-7296-4961-AB03-ED770F7D287B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Etude Structure Primaire" sheetId="1" r:id="rId1"/>
@@ -181,13 +181,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <i/>
       <sz val="11"/>
@@ -199,6 +192,14 @@
     <font>
       <i/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -357,19 +358,19 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -402,13 +403,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -963,10 +964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O64"/>
+  <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="C7" sqref="A7:C29"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:XFD60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -987,26 +988,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="J3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="35" t="s">
+      <c r="K3" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H6" s="5" t="s">
@@ -1772,15 +1773,9 @@
       <c r="D59" s="23"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B60" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C60" s="23" t="s">
-        <v>27</v>
-      </c>
+      <c r="A60" s="23"/>
+      <c r="B60" s="23"/>
+      <c r="C60" s="23"/>
       <c r="D60" s="23"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -1791,25 +1786,43 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="B62" s="23"/>
-      <c r="C62" s="23"/>
+        <v>25</v>
+      </c>
+      <c r="B62" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C62" s="23" t="s">
+        <v>27</v>
+      </c>
       <c r="D62" s="23"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="24">
-        <v>43724</v>
-      </c>
+      <c r="A63" s="23"/>
       <c r="B63" s="23"/>
       <c r="C63" s="23"/>
       <c r="D63" s="23"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B64" s="23"/>
+      <c r="C64" s="23"/>
+      <c r="D64" s="23"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="24">
+        <v>43724</v>
+      </c>
+      <c r="B65" s="23"/>
+      <c r="C65" s="23"/>
+      <c r="D65" s="23"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B64" s="23" t="s">
+      <c r="B66" s="23" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1884,7 +1897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B649AB-C754-4395-AD7A-03DF1FA37F74}">
   <dimension ref="B5:G21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
@@ -1899,22 +1912,22 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="G5" s="35" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MAJ pour Formation Frame - Re
</commit_message>
<xml_diff>
--- a/FR_Frame_Body/FR_A0100 (Frame)/Minimum Rules - Primary Structures.xlsx
+++ b/FR_Frame_Body/FR_A0100 (Frame)/Minimum Rules - Primary Structures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calixthe\Desktop\EPSA\STUF-2020\FR_Frame_Body\FR_A0100 (Frame)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CAD0B0-7296-4961-AB03-ED770F7D287B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2BF699-7D91-4FCA-B33B-66EA349A30AF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="35">
   <si>
     <t>Minimum requirements of frame</t>
   </si>
@@ -114,12 +114,6 @@
     <t>Fait par :</t>
   </si>
   <si>
-    <t>Robin CLAMENS</t>
-  </si>
-  <si>
-    <t>Calixthe MATTEI</t>
-  </si>
-  <si>
     <t>ULMTECHNOLOGIE</t>
   </si>
   <si>
@@ -132,9 +126,6 @@
     <t>2x + cher que 25x1,5</t>
   </si>
   <si>
-    <t>v2.1</t>
-  </si>
-  <si>
     <t>Véhicule</t>
   </si>
   <si>
@@ -142,6 +133,12 @@
   </si>
   <si>
     <t>Le plus optimal et autorisée par le règlement, dans le catalogue</t>
+  </si>
+  <si>
+    <t>Robin CLAMENS &amp; Calixthe MATTEI</t>
+  </si>
+  <si>
+    <t>v2.2</t>
   </si>
 </sst>
 </file>
@@ -299,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -410,6 +407,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -967,7 +967,7 @@
   <dimension ref="A1:O66"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60:XFD60"/>
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1788,13 +1788,11 @@
       <c r="A62" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B62" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C62" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D62" s="23"/>
+      <c r="B62" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C62" s="38"/>
+      <c r="D62" s="38"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="23"/>
@@ -1804,7 +1802,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="23" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B64" s="23"/>
       <c r="C64" s="23"/>
@@ -1812,7 +1810,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="24">
-        <v>43724</v>
+        <v>43925</v>
       </c>
       <c r="B65" s="23"/>
       <c r="C65" s="23"/>
@@ -1820,19 +1818,20 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B66" s="23" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:H33">
     <sortCondition ref="B7"/>
   </sortState>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="K3:M3"/>
     <mergeCell ref="D1:F2"/>
+    <mergeCell ref="B62:D62"/>
   </mergeCells>
   <conditionalFormatting sqref="J8">
     <cfRule type="cellIs" dxfId="14" priority="10" operator="greaterThan">
@@ -1925,7 +1924,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="35" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G5" s="35" t="s">
         <v>17</v>
@@ -2338,10 +2337,10 @@
   <sheetData>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="I3" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
@@ -2525,7 +2524,7 @@
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="26" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C11" s="27">
         <v>20</v>
@@ -2551,7 +2550,7 @@
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="26" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12" s="27">
         <v>20</v>
@@ -2751,10 +2750,10 @@
     </row>
     <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="33" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C20" s="28">
         <v>25</v>
@@ -2782,7 +2781,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B21" s="26" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C21" s="28">
         <v>25</v>
@@ -2954,7 +2953,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B28" s="26" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C28" s="28">
         <v>28</v>
@@ -2980,7 +2979,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B29" s="26" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C29" s="28">
         <v>28</v>
@@ -3056,7 +3055,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B32" s="26" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C32" s="28">
         <v>30</v>

</xml_diff>